<commit_message>
Added CDS All studies testcase
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC01_CDS_phs001437.xlsx
+++ b/InputFiles/CDS/TC01_CDS_phs001437.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0809\Commons_Automation\InputFiles\CDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0925\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1019C721-FFF3-44AA-8483-D315C64EE6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F97BBF3-959E-4112-950D-5B571CF5F3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>WebExcel</t>
   </si>
@@ -148,34 +148,6 @@
   </si>
   <si>
     <t>SELECT
-    DISTINCT (smp.sample_id) AS "Sample ID",
-    sp.participant_id AS "Participant ID", 
-    s.study_name AS "Study Name",
-    s.phs_accession AS Accession,
-    smp.sample_tumor_status AS Tumor,
-    smp.sample_type AS "Analyte Type"
-FROM 
-    df_participant sp
-JOIN 
-    df_study s ON sp."study.phs_accession" = s.phs_accession
-JOIN 
-    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
-JOIN
-    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
-JOIN
-    df_program p ON p.program_acronym = s."program.program_acronym"
-JOIN
-    df_file f1 ON f1."sample.sample_id" = smp.sample_id
-JOIN
-    df_genomic_info gi ON gi."file.file_id" = f1.file_id
-WHERE 
-    s.phs_accession = 'phs001437'
-ORDER BY 
-    smp.sample_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT
     f1.file_name AS "File Name",
     s.study_name AS "Study Name",
     s.phs_accession AS "Accession",
@@ -219,6 +191,32 @@
     gi.library_strategy
 ORDER BY 
     f1.file_name ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT
+    DISTINCT (smp.sample_id) AS "Sample ID",
+    sp.participant_id AS "Participant ID", 
+    s.study_name AS "Study Name",
+    s.phs_accession AS Accession
+FROM 
+    df_participant sp
+JOIN 
+    df_study s ON sp."study.phs_accession" = s.phs_accession
+JOIN 
+    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
+JOIN
+    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
+JOIN
+    df_program p ON p.program_acronym = s."program.program_acronym"
+JOIN
+    df_file f1 ON f1."sample.sample_id" = smp.sample_id
+JOIN
+    df_genomic_info gi ON gi."file.file_id" = f1.file_id
+WHERE 
+    s.phs_accession = 'phs001437'
+ORDER BY 
+    smp.sample_id ASC
 LIMIT 100;</t>
   </si>
 </sst>
@@ -611,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,30 +660,18 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>

</xml_diff>